<commit_message>
Added scripts for HIV AIDS mortality after HAART
</commit_message>
<xml_diff>
--- a/SaloniDattani/Antipsychotic-drugs/Psychosis medications historical dataset.xlsx
+++ b/SaloniDattani/Antipsychotic-drugs/Psychosis medications historical dataset.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>Treatment_name</t>
   </si>
@@ -32,6 +32,9 @@
     <t>Inventor_manufacturer_first</t>
   </si>
   <si>
+    <t>FDA_approved_generic_or_branded_2024</t>
+  </si>
+  <si>
     <t>Chlorpromazine</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
     <t>Paul Charpentier (original synthesis); Simone Courvoisier at Rhône Poulenc; Laborit, Lehmann, and Deniker (credited Lasker prize)</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Reserpine</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
     <t>Natural compound in the plant Rauvolfia serpentina; first synthesized by R. B. Woodward in 1958; first licensed as an antihypertensive in 1953 and as a tranquilizer/antipsychotic as 1954</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Perphenazine</t>
   </si>
   <si>
@@ -221,7 +230,7 @@
     <t>Otsuka Pharmaceutical / Lundbeck</t>
   </si>
   <si>
-    <t>Pimvanserin</t>
+    <t>Pimavanserin</t>
   </si>
   <si>
     <t>Acadia Pharmaceutical</t>
@@ -257,9 +266,6 @@
     <t>text, e.g. clozapine</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Subtype of treatment</t>
   </si>
   <si>
@@ -275,7 +281,7 @@
     <t>text, e.g. Phenothiazine</t>
   </si>
   <si>
-    <t>PubChem MeSH Tree classification</t>
+    <t>PubChem MeSH Tree classification (https://pubchem.ncbi.nlm.nih.gov/)</t>
   </si>
   <si>
     <t>The year it was first synthesized or developed in any country</t>
@@ -284,9 +290,6 @@
     <t>numeric, e.g. 1958</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>The year it was first approved in the United States</t>
   </si>
   <si>
@@ -300,6 +303,15 @@
   </si>
   <si>
     <t>text, e.g. Wander AG</t>
+  </si>
+  <si>
+    <t>Is the drug is still in use and approved by the FDA as of July 2024? (Note: includes any version, i.e. original brand drug or generic)</t>
+  </si>
+  <si>
+    <t>category, e.g. Yes or No</t>
+  </si>
+  <si>
+    <t>Drugs@FDA (https://www.accessdata.fda.gov/scripts/cder/daf/)</t>
   </si>
 </sst>
 </file>
@@ -571,9 +583,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.25"/>
     <col customWidth="1" min="2" max="2" width="25.13"/>
-    <col customWidth="1" min="3" max="4" width="19.0"/>
+    <col customWidth="1" min="3" max="3" width="19.88"/>
+    <col customWidth="1" min="4" max="4" width="19.0"/>
     <col customWidth="1" min="5" max="5" width="25.13"/>
-    <col customWidth="1" min="6" max="6" width="25.38"/>
+    <col customWidth="1" min="6" max="6" width="23.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -595,16 +608,20 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>1950.0</v>
@@ -613,18 +630,21 @@
         <v>1954.0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <v>1958.0</v>
@@ -633,54 +653,63 @@
         <v>1954.0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
         <v>1957.0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
         <v>1957.0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>1958.0</v>
@@ -689,126 +718,147 @@
         <v>1958.0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
         <v>1959.0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
         <v>1959.0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
         <v>1967.0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
         <v>1971.0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
         <v>1974.0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <v>1976.0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2">
         <v>1958.0</v>
@@ -817,18 +867,21 @@
         <v>1990.0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
         <v>1985.0</v>
@@ -837,211 +890,250 @@
         <v>1994.0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2">
         <v>1996.0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E16" s="2">
         <v>1997.0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2">
         <v>1997.0</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E18" s="2">
         <v>2002.0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2">
         <v>2006.0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E20" s="2">
         <v>2009.0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E21" s="2">
         <v>2009.0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E22" s="2">
         <v>2010.0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E23" s="2">
         <v>2015.0</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2">
         <v>2015.0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E25" s="2">
         <v>2016.0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2">
         <v>2019.0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1067,19 +1159,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
@@ -1087,13 +1179,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -1101,16 +1193,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
@@ -1118,16 +1210,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -1135,16 +1227,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
@@ -1152,16 +1244,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -1169,16 +1261,33 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>